<commit_message>
GQA e GRE - end
</commit_message>
<xml_diff>
--- a/Raiz/Processo/Avaliação/GQA-Avaliação Processo.xlsx
+++ b/Raiz/Processo/Avaliação/GQA-Avaliação Processo.xlsx
@@ -1470,8 +1470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2124,17 +2124,17 @@
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
     <hyperlink ref="C20" r:id="rId1"/>
-    <hyperlink ref="C28" r:id="rId2"/>
-    <hyperlink ref="C29" r:id="rId3"/>
-    <hyperlink ref="C39" r:id="rId4"/>
-    <hyperlink ref="C74" r:id="rId5"/>
-    <hyperlink ref="C60" r:id="rId6"/>
-    <hyperlink ref="C53" r:id="rId7"/>
-    <hyperlink ref="C46" r:id="rId8"/>
-    <hyperlink ref="C6" r:id="rId9"/>
-    <hyperlink ref="C67" r:id="rId10"/>
-    <hyperlink ref="C13" r:id="rId11"/>
-    <hyperlink ref="C81" r:id="rId12"/>
+    <hyperlink ref="C29" r:id="rId2"/>
+    <hyperlink ref="C6" r:id="rId3"/>
+    <hyperlink ref="C67" r:id="rId4"/>
+    <hyperlink ref="C13" r:id="rId5"/>
+    <hyperlink ref="C81" r:id="rId6"/>
+    <hyperlink ref="C28" r:id="rId7"/>
+    <hyperlink ref="C39" r:id="rId8"/>
+    <hyperlink ref="C46" r:id="rId9"/>
+    <hyperlink ref="C53" r:id="rId10"/>
+    <hyperlink ref="C60" r:id="rId11"/>
+    <hyperlink ref="C74" r:id="rId12"/>
     <hyperlink ref="C54" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>

</xml_diff>